<commit_message>
fix the way to retrieve assign site
</commit_message>
<xml_diff>
--- a/docs/needAdjust.xlsx
+++ b/docs/needAdjust.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="30" uniqueCount="26">
   <si>
     <t>CustomerID</t>
   </si>
@@ -25,22 +25,73 @@
     <t>CustomerAddress</t>
   </si>
   <si>
-    <t>85CAFE1030001747</t>
-  </si>
-  <si>
-    <t>77777</t>
-  </si>
-  <si>
-    <t>85度C  南科群創店</t>
-  </si>
-  <si>
-    <t>鋼鐵韓粉</t>
-  </si>
-  <si>
-    <t>台南市新市市環西路一段3號</t>
-  </si>
-  <si>
-    <t>雲林縣斗六夜市</t>
+    <t>POST009112-5</t>
+  </si>
+  <si>
+    <t>POST014122-5</t>
+  </si>
+  <si>
+    <t>SET180632</t>
+  </si>
+  <si>
+    <t>TCAT009203</t>
+  </si>
+  <si>
+    <t>TCAT223010</t>
+  </si>
+  <si>
+    <t>TCATOA223010</t>
+  </si>
+  <si>
+    <t>TRA057</t>
+  </si>
+  <si>
+    <t>TRA057出入</t>
+  </si>
+  <si>
+    <t>TRA375</t>
+  </si>
+  <si>
+    <t>秀林和平郵局(花蓮12支)</t>
+  </si>
+  <si>
+    <t>和平梨山郵局(台中94支)</t>
+  </si>
+  <si>
+    <t>統一超商  環山店</t>
+  </si>
+  <si>
+    <t>統一速達    梨山衛星所</t>
+  </si>
+  <si>
+    <t>統一速達  梨山衛星所</t>
+  </si>
+  <si>
+    <t>台灣鐵路管理局　和平站</t>
+  </si>
+  <si>
+    <t>台灣鐵路管理局　和平站  出入口</t>
+  </si>
+  <si>
+    <t>台灣鐵路管理局  阿里山站</t>
+  </si>
+  <si>
+    <t>花蓮縣秀林鄉和平村113號</t>
+  </si>
+  <si>
+    <t>台中市和平區梨山村中正路89號</t>
+  </si>
+  <si>
+    <t>台中市和平區中興路三段64-5、64-6號</t>
+  </si>
+  <si>
+    <t>台中市和平區梨山村福壽路5號之1</t>
+  </si>
+  <si>
+    <t>花蓮縣秀林鄉和平村２７６號</t>
+  </si>
+  <si>
+    <t>嘉義縣阿里山鄉中正村1號</t>
   </si>
 </sst>
 </file>
@@ -398,7 +449,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:C3"/>
+  <dimension ref="A1:C10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -420,10 +471,10 @@
         <v>3</v>
       </c>
       <c r="B2" t="s">
-        <v>5</v>
+        <v>12</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>20</v>
       </c>
     </row>
     <row r="3" spans="1:3">
@@ -431,10 +482,87 @@
         <v>4</v>
       </c>
       <c r="B3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3">
+      <c r="A4" t="s">
+        <v>5</v>
+      </c>
+      <c r="B4" t="s">
+        <v>14</v>
+      </c>
+      <c r="C4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3">
+      <c r="A5" t="s">
         <v>6</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B5" t="s">
+        <v>15</v>
+      </c>
+      <c r="C5" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3">
+      <c r="A6" t="s">
+        <v>7</v>
+      </c>
+      <c r="B6" t="s">
+        <v>16</v>
+      </c>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3">
+      <c r="A7" t="s">
         <v>8</v>
+      </c>
+      <c r="B7" t="s">
+        <v>16</v>
+      </c>
+      <c r="C7" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3">
+      <c r="A8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B8" t="s">
+        <v>17</v>
+      </c>
+      <c r="C8" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3">
+      <c r="A9" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" t="s">
+        <v>18</v>
+      </c>
+      <c r="C9" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3">
+      <c r="A10" t="s">
+        <v>11</v>
+      </c>
+      <c r="B10" t="s">
+        <v>19</v>
+      </c>
+      <c r="C10" t="s">
+        <v>25</v>
       </c>
     </row>
   </sheetData>

</xml_diff>